<commit_message>
add multiple colors for tables
</commit_message>
<xml_diff>
--- a/example/sample_datamodel.xlsx
+++ b/example/sample_datamodel.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnaudrover/PycharmProjects/pdm_diagram/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnaudrover/PycharmProjects/pdm_diagram/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6375A472-D915-FB46-B32E-F35CF0CBEC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22347C8F-77F1-264E-A0F6-67D5E61CC5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="4620" windowWidth="23260" windowHeight="12580" activeTab="7" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
+    <workbookView xWindow="5300" yWindow="4620" windowWidth="23260" windowHeight="12580" firstSheet="1" activeTab="8" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
   </bookViews>
   <sheets>
     <sheet name="table merchants" sheetId="4" r:id="rId1"/>
     <sheet name="table users" sheetId="5" r:id="rId2"/>
-    <sheet name="table countries" sheetId="6" r:id="rId3"/>
-    <sheet name="table order_items" sheetId="7" r:id="rId4"/>
+    <sheet name="table_ref countries" sheetId="6" r:id="rId3"/>
+    <sheet name="table_rel order_items" sheetId="7" r:id="rId4"/>
     <sheet name="table orders" sheetId="8" r:id="rId5"/>
     <sheet name="table products" sheetId="9" r:id="rId6"/>
     <sheet name="table merchant_periods" sheetId="10" r:id="rId7"/>
     <sheet name="table product_tags" sheetId="11" r:id="rId8"/>
+    <sheet name="ignore table" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -223,8 +224,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,7 +233,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -264,9 +271,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -287,7 +291,7 @@
     <tableColumn id="1" xr3:uid="{7D9740D5-949A-467E-A4DA-59CD6F496B73}" name="pk"/>
     <tableColumn id="5" xr3:uid="{6146C0F0-DBDD-4207-8E89-9DAC2B6B28EE}" name="fk"/>
     <tableColumn id="7" xr3:uid="{D28B7764-E64E-014B-81C9-DD3C182ADF06}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{23E5011F-AE7B-42CA-800F-EE73D269C13C}" name="name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{23E5011F-AE7B-42CA-800F-EE73D269C13C}" name="name" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{B9E48BC1-B016-4F43-84B4-28D4B7706034}" name="type"/>
     <tableColumn id="6" xr3:uid="{7B4B9390-CB0B-4B4B-8657-FE27CF279033}" name="Description"/>
     <tableColumn id="4" xr3:uid="{9CBB7A64-4A89-4783-BE75-573145A6FBEF}" name="Exemple"/>
@@ -319,7 +323,7 @@
     <tableColumn id="1" xr3:uid="{9A2B64F8-88CD-CE49-80E6-370EFB92073C}" name="pk"/>
     <tableColumn id="5" xr3:uid="{FC761FB0-C872-394E-9D62-4A71A6C17CED}" name="fk"/>
     <tableColumn id="7" xr3:uid="{A9B217BA-5CC6-FD4D-8669-3E0239908479}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{D8B3C2A9-BE83-6E46-9EF4-D307B0F0EC15}" name="name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{D8B3C2A9-BE83-6E46-9EF4-D307B0F0EC15}" name="name" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{1E78BFD1-5C3C-7B44-B35A-5B82025B0587}" name="type"/>
     <tableColumn id="6" xr3:uid="{2785C3C9-45FD-E949-B384-D16E76340559}" name="Description"/>
     <tableColumn id="4" xr3:uid="{39A0662C-CA0B-2D4A-83BA-D07DF5F8C1EF}" name="Exemple"/>
@@ -335,7 +339,7 @@
     <tableColumn id="1" xr3:uid="{1E7295F7-D2A5-E148-99E3-2C6470221F87}" name="pk"/>
     <tableColumn id="5" xr3:uid="{9E10E9E7-24A3-C541-96FB-F242EAFE5715}" name="fk"/>
     <tableColumn id="7" xr3:uid="{9F13C0DE-AE3C-384C-AF85-512B7059335C}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{09E214A8-490E-894B-B9C6-C879A61CC2B6}" name="name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{09E214A8-490E-894B-B9C6-C879A61CC2B6}" name="name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{21CAF3C5-1617-5240-A683-03D85122026B}" name="type"/>
     <tableColumn id="6" xr3:uid="{FDEAFCBB-A4F0-214D-B1DF-14054729A906}" name="Description"/>
     <tableColumn id="4" xr3:uid="{9336C418-8D6C-D044-AB63-801AF22D6278}" name="Exemple"/>
@@ -351,7 +355,7 @@
     <tableColumn id="1" xr3:uid="{4E0645E4-9C72-B042-A371-B2DA4EEC5CF5}" name="pk"/>
     <tableColumn id="5" xr3:uid="{1DB5E8B3-C125-C941-9A0B-29FD2399A4E1}" name="fk"/>
     <tableColumn id="7" xr3:uid="{C1195102-8860-A447-8B04-4523E588715C}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{27F4113D-BE4D-8F4C-8074-14D34BC189EE}" name="name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{27F4113D-BE4D-8F4C-8074-14D34BC189EE}" name="name" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{794810E0-6AB9-1F49-8EC4-E19181EADED0}" name="type"/>
     <tableColumn id="6" xr3:uid="{682DEA62-9478-EC45-918D-13570680B917}" name="Description"/>
     <tableColumn id="4" xr3:uid="{4862001A-4EA1-9C4A-94CF-E9440DDF91D0}" name="Exemple"/>
@@ -367,7 +371,7 @@
     <tableColumn id="1" xr3:uid="{EAA659E1-98E1-6C4F-A8AA-455E6D6F0E6C}" name="pk"/>
     <tableColumn id="5" xr3:uid="{CBFC82CB-D2B3-7641-9EE9-652935D06E65}" name="fk"/>
     <tableColumn id="7" xr3:uid="{86D7A8E5-F07C-3148-81CB-96EC52225F9E}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{38CD1CB2-8289-DE45-824F-E36ED0F4B240}" name="name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{38CD1CB2-8289-DE45-824F-E36ED0F4B240}" name="name" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{CC157D6C-14AD-5E49-B18B-2CB8EAA24100}" name="type"/>
     <tableColumn id="6" xr3:uid="{959D5BD0-1E1D-5C47-BA0E-69457902550E}" name="Description"/>
     <tableColumn id="4" xr3:uid="{AC7C8AE6-7DA9-A04D-99B5-3B3BB02748CA}" name="Exemple"/>
@@ -383,7 +387,7 @@
     <tableColumn id="1" xr3:uid="{D8C19591-6C2B-A342-8DA4-675F7C607A96}" name="pk"/>
     <tableColumn id="5" xr3:uid="{06351AD1-7539-D84D-A810-05ADF45109BD}" name="fk"/>
     <tableColumn id="7" xr3:uid="{CD6843D2-7B99-DB4B-AEC7-5E9EEE2E0CC2}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{8A057813-083D-9C41-A66F-096F3579F098}" name="name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8A057813-083D-9C41-A66F-096F3579F098}" name="name" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{FB3FD6C7-24CC-4C4D-A206-B61B1C460547}" name="type"/>
     <tableColumn id="6" xr3:uid="{3F4EB876-28B8-FB44-9500-83E514DC8742}" name="Description"/>
     <tableColumn id="4" xr3:uid="{62F5AFC6-74C1-BE41-BB3C-BE34B3C56BC9}" name="Exemple"/>
@@ -399,10 +403,26 @@
     <tableColumn id="1" xr3:uid="{AB1F73F4-EAF0-3F46-861D-97D754EA70F7}" name="pk"/>
     <tableColumn id="5" xr3:uid="{D46BF95F-89ED-804F-9F91-A18D9F0383CF}" name="fk"/>
     <tableColumn id="7" xr3:uid="{ADEBDA1D-1203-C944-953D-7093B1CF25F4}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{971B5AA5-C6D9-644F-B393-6B0E52239D7D}" name="name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{971B5AA5-C6D9-644F-B393-6B0E52239D7D}" name="name" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{E19CD575-5C16-6048-9713-4F5069CD0B59}" name="type"/>
     <tableColumn id="6" xr3:uid="{9F12CA64-5DEA-774B-AD1B-718AE1195641}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00D44D73-7E45-C045-9C09-4CC254EE5C82}" name="Exemple"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}" name="Tableau3623578910" displayName="Tableau3623578910" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4D2A244F-89D1-8A4A-B799-27B551D67073}" name="pk"/>
+    <tableColumn id="5" xr3:uid="{DFDE1DB2-CBC6-C242-B967-55EB652C3939}" name="fk"/>
+    <tableColumn id="7" xr3:uid="{664628BB-E798-BD48-B503-ECCFAF790801}" name="nullable"/>
+    <tableColumn id="2" xr3:uid="{75263241-203E-1540-B2CD-3FD9CC27C5FA}" name="name" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1C6941EF-8554-4741-9AEF-35096FD37E34}" name="type"/>
+    <tableColumn id="6" xr3:uid="{C44CB72C-C1BD-A846-8D87-307C94C44E31}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{FEFE3B91-C554-684A-A20D-839F09D1686D}" name="Exemple"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1442,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B448C70-C7FF-4942-B374-2EDF264F54A9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1517,27 +1537,86 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F7C29-4F3B-1249-A948-CD711F55882F}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27b5a61b-5e22-4594-9140-9e3611d4b7f6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c4c029f3-007d-4fee-b932-408a6e0f9385" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F907AAAB01E0CA47914A53F4D022691C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="789b62fba9185e274c939cd4060d44f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27b5a61b-5e22-4594-9140-9e3611d4b7f6" xmlns:ns3="c4c029f3-007d-4fee-b932-408a6e0f9385" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86bb8fd1e3132d8e8f130ed8c8e6d9b5" ns2:_="" ns3:_="">
     <xsd:import namespace="27b5a61b-5e22-4594-9140-9e3611d4b7f6"/>
@@ -1748,26 +1827,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27b5a61b-5e22-4594-9140-9e3611d4b7f6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c4c029f3-007d-4fee-b932-408a6e0f9385" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76DCE868-386D-4D20-9AAF-DBEC6C765C65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27b5a61b-5e22-4594-9140-9e3611d4b7f6"/>
-    <ds:schemaRef ds:uri="c4c029f3-007d-4fee-b932-408a6e0f9385"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74FECA5F-B77A-4F71-AA2C-506B17262806}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5C43E4-AC7B-43FA-A6BF-9EEF3AEE0A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1784,4 +1864,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74FECA5F-B77A-4F71-AA2C-506B17262806}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76DCE868-386D-4D20-9AAF-DBEC6C765C65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27b5a61b-5e22-4594-9140-9e3611d4b7f6"/>
+    <ds:schemaRef ds:uri="c4c029f3-007d-4fee-b932-408a6e0f9385"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding support of PK also FK
</commit_message>
<xml_diff>
--- a/example/sample_datamodel.xlsx
+++ b/example/sample_datamodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnaudrover/PycharmProjects/pdm_diagram/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5E7DF5-4FD3-3242-B11D-F2AAEE4F6631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BFBBA1-76B0-8E48-A44A-9E5FC92E5AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="5120" windowWidth="23260" windowHeight="10180" activeTab="3" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
+    <workbookView xWindow="2340" yWindow="5120" windowWidth="23260" windowHeight="10180" activeTab="6" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
   </bookViews>
   <sheets>
     <sheet name="table merchants" sheetId="4" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="table_rel order_items" sheetId="7" r:id="rId4"/>
     <sheet name="table orders" sheetId="8" r:id="rId5"/>
     <sheet name="table products" sheetId="9" r:id="rId6"/>
-    <sheet name="table merchant_periods" sheetId="10" r:id="rId7"/>
-    <sheet name="table product_tags" sheetId="11" r:id="rId8"/>
-    <sheet name="ignore table" sheetId="12" r:id="rId9"/>
+    <sheet name="table product_details" sheetId="13" r:id="rId7"/>
+    <sheet name="table merchant_periods" sheetId="10" r:id="rId8"/>
+    <sheet name="table product_tags" sheetId="11" r:id="rId9"/>
+    <sheet name="ignore table" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -157,6 +158,18 @@
   </si>
   <si>
     <t>FK products.id 0n:1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>FK products.id 01:11</t>
   </si>
 </sst>
 </file>
@@ -242,7 +255,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -300,10 +316,26 @@
     <tableColumn id="1" xr3:uid="{7D9740D5-949A-467E-A4DA-59CD6F496B73}" name="pk"/>
     <tableColumn id="5" xr3:uid="{6146C0F0-DBDD-4207-8E89-9DAC2B6B28EE}" name="fk"/>
     <tableColumn id="7" xr3:uid="{D28B7764-E64E-014B-81C9-DD3C182ADF06}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{23E5011F-AE7B-42CA-800F-EE73D269C13C}" name="name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{23E5011F-AE7B-42CA-800F-EE73D269C13C}" name="name" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{B9E48BC1-B016-4F43-84B4-28D4B7706034}" name="type"/>
     <tableColumn id="6" xr3:uid="{7B4B9390-CB0B-4B4B-8657-FE27CF279033}" name="Description"/>
     <tableColumn id="4" xr3:uid="{9CBB7A64-4A89-4783-BE75-573145A6FBEF}" name="Exemple"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}" name="Tableau3623578910" displayName="Tableau3623578910" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4D2A244F-89D1-8A4A-B799-27B551D67073}" name="pk"/>
+    <tableColumn id="5" xr3:uid="{DFDE1DB2-CBC6-C242-B967-55EB652C3939}" name="fk"/>
+    <tableColumn id="7" xr3:uid="{664628BB-E798-BD48-B503-ECCFAF790801}" name="nullable"/>
+    <tableColumn id="2" xr3:uid="{75263241-203E-1540-B2CD-3FD9CC27C5FA}" name="name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1C6941EF-8554-4741-9AEF-35096FD37E34}" name="type"/>
+    <tableColumn id="6" xr3:uid="{C44CB72C-C1BD-A846-8D87-307C94C44E31}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{FEFE3B91-C554-684A-A20D-839F09D1686D}" name="Exemple"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -316,7 +348,7 @@
     <tableColumn id="1" xr3:uid="{823D52DE-9C80-41E5-8F4D-3D5FACCA27C5}" name="pk"/>
     <tableColumn id="5" xr3:uid="{B03E5154-F689-47CF-8DC3-4BF67A4EC0EF}" name="fk"/>
     <tableColumn id="7" xr3:uid="{F418E029-8FC5-B14B-B7DF-3857826960FA}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{8D83A9F5-9037-4CEC-AA7D-357994AF79BE}" name="name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8D83A9F5-9037-4CEC-AA7D-357994AF79BE}" name="name" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{C15DFD6C-FE94-4ECD-92A3-0B8D24D4D638}" name="type"/>
     <tableColumn id="6" xr3:uid="{AB397DC0-6903-4510-9DE9-E86BB6B89BD6}" name="Description"/>
     <tableColumn id="4" xr3:uid="{545831CE-0A2B-4FD4-8D79-08D5A641FACF}" name="Exemple"/>
@@ -332,7 +364,7 @@
     <tableColumn id="1" xr3:uid="{9A2B64F8-88CD-CE49-80E6-370EFB92073C}" name="pk"/>
     <tableColumn id="5" xr3:uid="{FC761FB0-C872-394E-9D62-4A71A6C17CED}" name="fk"/>
     <tableColumn id="7" xr3:uid="{A9B217BA-5CC6-FD4D-8669-3E0239908479}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{D8B3C2A9-BE83-6E46-9EF4-D307B0F0EC15}" name="name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D8B3C2A9-BE83-6E46-9EF4-D307B0F0EC15}" name="name" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{1E78BFD1-5C3C-7B44-B35A-5B82025B0587}" name="type"/>
     <tableColumn id="6" xr3:uid="{2785C3C9-45FD-E949-B384-D16E76340559}" name="Description"/>
     <tableColumn id="4" xr3:uid="{39A0662C-CA0B-2D4A-83BA-D07DF5F8C1EF}" name="Exemple"/>
@@ -348,7 +380,7 @@
     <tableColumn id="1" xr3:uid="{1E7295F7-D2A5-E148-99E3-2C6470221F87}" name="pk"/>
     <tableColumn id="5" xr3:uid="{9E10E9E7-24A3-C541-96FB-F242EAFE5715}" name="fk"/>
     <tableColumn id="7" xr3:uid="{9F13C0DE-AE3C-384C-AF85-512B7059335C}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{09E214A8-490E-894B-B9C6-C879A61CC2B6}" name="name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{09E214A8-490E-894B-B9C6-C879A61CC2B6}" name="name" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{21CAF3C5-1617-5240-A683-03D85122026B}" name="type"/>
     <tableColumn id="6" xr3:uid="{FDEAFCBB-A4F0-214D-B1DF-14054729A906}" name="Description"/>
     <tableColumn id="4" xr3:uid="{9336C418-8D6C-D044-AB63-801AF22D6278}" name="Exemple"/>
@@ -364,7 +396,7 @@
     <tableColumn id="1" xr3:uid="{4E0645E4-9C72-B042-A371-B2DA4EEC5CF5}" name="pk"/>
     <tableColumn id="5" xr3:uid="{1DB5E8B3-C125-C941-9A0B-29FD2399A4E1}" name="fk"/>
     <tableColumn id="7" xr3:uid="{C1195102-8860-A447-8B04-4523E588715C}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{27F4113D-BE4D-8F4C-8074-14D34BC189EE}" name="name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{27F4113D-BE4D-8F4C-8074-14D34BC189EE}" name="name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{794810E0-6AB9-1F49-8EC4-E19181EADED0}" name="type"/>
     <tableColumn id="6" xr3:uid="{682DEA62-9478-EC45-918D-13570680B917}" name="Description"/>
     <tableColumn id="4" xr3:uid="{4862001A-4EA1-9C4A-94CF-E9440DDF91D0}" name="Exemple"/>
@@ -380,7 +412,7 @@
     <tableColumn id="1" xr3:uid="{EAA659E1-98E1-6C4F-A8AA-455E6D6F0E6C}" name="pk"/>
     <tableColumn id="5" xr3:uid="{CBFC82CB-D2B3-7641-9EE9-652935D06E65}" name="fk"/>
     <tableColumn id="7" xr3:uid="{86D7A8E5-F07C-3148-81CB-96EC52225F9E}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{38CD1CB2-8289-DE45-824F-E36ED0F4B240}" name="name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{38CD1CB2-8289-DE45-824F-E36ED0F4B240}" name="name" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{CC157D6C-14AD-5E49-B18B-2CB8EAA24100}" name="type"/>
     <tableColumn id="6" xr3:uid="{959D5BD0-1E1D-5C47-BA0E-69457902550E}" name="Description"/>
     <tableColumn id="4" xr3:uid="{AC7C8AE6-7DA9-A04D-99B5-3B3BB02748CA}" name="Exemple"/>
@@ -390,13 +422,29 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{65634D0E-A46D-6547-A6BB-E8662E03015B}" name="Tableau36235711" displayName="Tableau36235711" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{65634D0E-A46D-6547-A6BB-E8662E03015B}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{56D07ED8-A3A5-6B42-8F57-9E104D5AE9F3}" name="pk"/>
+    <tableColumn id="5" xr3:uid="{91F2F706-8343-5E4E-8E87-329C23C86505}" name="fk"/>
+    <tableColumn id="7" xr3:uid="{9F3C824B-EA1A-B042-A7EA-B2DF0A46B2B1}" name="nullable"/>
+    <tableColumn id="2" xr3:uid="{611D5096-C9EF-1C44-8725-152847CBC4B6}" name="name" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{4EAA440C-59BC-B44E-90A6-E014E663BB5B}" name="type"/>
+    <tableColumn id="6" xr3:uid="{60E85D8D-E870-F64A-A0F6-2327DA9C55EF}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{E64B309F-C789-6A41-860B-C89E28069E3A}" name="Exemple"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{732977BE-D06D-9C45-A29B-015E4AF67033}" name="Tableau3623578" displayName="Tableau3623578" ref="A1:G14" totalsRowShown="0">
   <autoFilter ref="A1:G14" xr:uid="{732977BE-D06D-9C45-A29B-015E4AF67033}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D8C19591-6C2B-A342-8DA4-675F7C607A96}" name="pk"/>
     <tableColumn id="5" xr3:uid="{06351AD1-7539-D84D-A810-05ADF45109BD}" name="fk"/>
     <tableColumn id="7" xr3:uid="{CD6843D2-7B99-DB4B-AEC7-5E9EEE2E0CC2}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{8A057813-083D-9C41-A66F-096F3579F098}" name="name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{8A057813-083D-9C41-A66F-096F3579F098}" name="name" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{FB3FD6C7-24CC-4C4D-A206-B61B1C460547}" name="type"/>
     <tableColumn id="6" xr3:uid="{3F4EB876-28B8-FB44-9500-83E514DC8742}" name="Description"/>
     <tableColumn id="4" xr3:uid="{62F5AFC6-74C1-BE41-BB3C-BE34B3C56BC9}" name="Exemple"/>
@@ -405,33 +453,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{08E178EC-7DDE-654F-B5C2-FFD2FA20090A}" name="Tableau36235789" displayName="Tableau36235789" ref="A1:G14" totalsRowShown="0">
   <autoFilter ref="A1:G14" xr:uid="{08E178EC-7DDE-654F-B5C2-FFD2FA20090A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AB1F73F4-EAF0-3F46-861D-97D754EA70F7}" name="pk"/>
     <tableColumn id="5" xr3:uid="{D46BF95F-89ED-804F-9F91-A18D9F0383CF}" name="fk"/>
     <tableColumn id="7" xr3:uid="{ADEBDA1D-1203-C944-953D-7093B1CF25F4}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{971B5AA5-C6D9-644F-B393-6B0E52239D7D}" name="name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{971B5AA5-C6D9-644F-B393-6B0E52239D7D}" name="name" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{E19CD575-5C16-6048-9713-4F5069CD0B59}" name="type"/>
     <tableColumn id="6" xr3:uid="{9F12CA64-5DEA-774B-AD1B-718AE1195641}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00D44D73-7E45-C045-9C09-4CC254EE5C82}" name="Exemple"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}" name="Tableau3623578910" displayName="Tableau3623578910" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14" xr:uid="{AE88F8D4-BFB1-B544-AF1E-3F1E4CC63013}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D2A244F-89D1-8A4A-B799-27B551D67073}" name="pk"/>
-    <tableColumn id="5" xr3:uid="{DFDE1DB2-CBC6-C242-B967-55EB652C3939}" name="fk"/>
-    <tableColumn id="7" xr3:uid="{664628BB-E798-BD48-B503-ECCFAF790801}" name="nullable"/>
-    <tableColumn id="2" xr3:uid="{75263241-203E-1540-B2CD-3FD9CC27C5FA}" name="name" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{1C6941EF-8554-4741-9AEF-35096FD37E34}" name="type"/>
-    <tableColumn id="6" xr3:uid="{C44CB72C-C1BD-A846-8D87-307C94C44E31}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{FEFE3B91-C554-684A-A20D-839F09D1686D}" name="Exemple"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,6 +881,85 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F7C29-4F3B-1249-A948-CD711F55882F}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFC174A-B6E9-4849-B9D2-031CD0AECDEE}">
   <dimension ref="A1:G6"/>
@@ -1046,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BA00AE-5915-5A48-BC98-02A1447C6DED}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1235,7 +1346,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1348,6 +1459,100 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9966FB-677D-D146-BD7E-AB0A74CAA3E8}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1107C318-2D2F-FA49-B3F6-91CE77D4463C}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1467,7 +1672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B448C70-C7FF-4942-B374-2EDF264F54A9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1546,92 +1751,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F7C29-4F3B-1249-A948-CD711F55882F}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D4" s="4"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D5" s="4"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-      <c r="G6" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27b5a61b-5e22-4594-9140-9e3611d4b7f6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c4c029f3-007d-4fee-b932-408a6e0f9385" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1846,20 +1974,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27b5a61b-5e22-4594-9140-9e3611d4b7f6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c4c029f3-007d-4fee-b932-408a6e0f9385" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74FECA5F-B77A-4F71-AA2C-506B17262806}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76DCE868-386D-4D20-9AAF-DBEC6C765C65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27b5a61b-5e22-4594-9140-9e3611d4b7f6"/>
+    <ds:schemaRef ds:uri="c4c029f3-007d-4fee-b932-408a6e0f9385"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1884,12 +2013,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76DCE868-386D-4D20-9AAF-DBEC6C765C65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74FECA5F-B77A-4F71-AA2C-506B17262806}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27b5a61b-5e22-4594-9140-9e3611d4b7f6"/>
-    <ds:schemaRef ds:uri="c4c029f3-007d-4fee-b932-408a6e0f9385"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add feature to hide columns
</commit_message>
<xml_diff>
--- a/example/sample_datamodel.xlsx
+++ b/example/sample_datamodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnaudrover/PycharmProjects/pdm_diagram/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BFBBA1-76B0-8E48-A44A-9E5FC92E5AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08693778-73D6-4749-BA1B-F482B4EE33F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="5120" windowWidth="23260" windowHeight="10180" activeTab="6" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
+    <workbookView xWindow="2340" yWindow="5120" windowWidth="23260" windowHeight="10180" activeTab="4" xr2:uid="{B43F630A-AB27-4473-8F56-4A58B33F5972}"/>
   </bookViews>
   <sheets>
     <sheet name="table merchants" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>FK products.id 01:11</t>
+  </si>
+  <si>
+    <t>col_hidden:h</t>
+  </si>
+  <si>
+    <t>col_hidden_logical:</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -251,6 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,8 +397,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C81938D0-B8C8-FB4C-A0F0-EA140B49F791}" name="Tableau36235" displayName="Tableau36235" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14" xr:uid="{C81938D0-B8C8-FB4C-A0F0-EA140B49F791}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C81938D0-B8C8-FB4C-A0F0-EA140B49F791}" name="Tableau36235" displayName="Tableau36235" ref="A1:G15" totalsRowShown="0">
+  <autoFilter ref="A1:G15" xr:uid="{C81938D0-B8C8-FB4C-A0F0-EA140B49F791}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4E0645E4-9C72-B042-A371-B2DA4EEC5CF5}" name="pk"/>
     <tableColumn id="5" xr3:uid="{1DB5E8B3-C125-C941-9A0B-29FD2399A4E1}" name="fk"/>
@@ -1245,13 +1252,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BDE393-3FD4-FD47-9BB9-EE4E991D41F6}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1321,17 +1331,37 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-      <c r="G6" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9966FB-677D-D146-BD7E-AB0A74CAA3E8}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>